<commit_message>
Update Documentation Datenanalyse Viren
</commit_message>
<xml_diff>
--- a/documentation/DatenAnalyse Viren.xlsx
+++ b/documentation/DatenAnalyse Viren.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="14115" windowHeight="7740" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="14115" windowHeight="7740" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -702,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -747,7 +747,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -763,6 +762,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1050,11 +1051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45446784"/>
-        <c:axId val="45447360"/>
+        <c:axId val="51779776"/>
+        <c:axId val="51780352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45446784"/>
+        <c:axId val="51779776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000"/>
@@ -1065,12 +1066,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45447360"/>
+        <c:crossAx val="51780352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45447360"/>
+        <c:axId val="51780352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45446784"/>
+        <c:crossAx val="51779776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1117,7 +1118,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1435,11 +1435,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98869824"/>
-        <c:axId val="98870400"/>
+        <c:axId val="44795008"/>
+        <c:axId val="44795584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98869824"/>
+        <c:axId val="44795008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,12 +1449,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98870400"/>
+        <c:crossAx val="44795584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98870400"/>
+        <c:axId val="44795584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,14 +1465,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98869824"/>
+        <c:crossAx val="44795008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1502,7 +1501,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1692,11 +1690,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115388416"/>
-        <c:axId val="98872128"/>
+        <c:axId val="45006336"/>
+        <c:axId val="44797312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115388416"/>
+        <c:axId val="45006336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98872128"/>
+        <c:crossAx val="44797312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1713,7 +1711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98872128"/>
+        <c:axId val="44797312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1724,14 +1722,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115388416"/>
+        <c:crossAx val="45006336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2245,11 +2242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98873856"/>
-        <c:axId val="98874432"/>
+        <c:axId val="44799040"/>
+        <c:axId val="44799616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98873856"/>
+        <c:axId val="44799040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000"/>
@@ -2260,12 +2257,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98874432"/>
+        <c:crossAx val="44799616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98874432"/>
+        <c:axId val="44799616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98873856"/>
+        <c:crossAx val="44799040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4617,8 +4614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4633,27 +4630,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="41"/>
+      <c r="A1" s="40"/>
       <c r="B1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
       <c r="G1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="9" t="s">
         <v>102</v>
       </c>
       <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="39" t="s">
         <v>135</v>
       </c>
       <c r="M2" t="s">
@@ -4676,8 +4673,8 @@
       <c r="G3" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="36">
-        <v>0.5</v>
+      <c r="H3" s="51">
+        <v>433.5</v>
       </c>
       <c r="K3" t="s">
         <v>143</v>
@@ -4739,15 +4736,15 @@
         <v>132</v>
       </c>
       <c r="M6" s="13">
-        <f>H3*M4</f>
+        <f>H3*M3</f>
         <v>426603.13828915579</v>
       </c>
       <c r="N6" s="13">
-        <f>H3*N4</f>
+        <f>H3*N3</f>
         <v>223975.59175212128</v>
       </c>
       <c r="O6" s="13">
-        <f>H3*O4</f>
+        <f>H3*O3</f>
         <v>139751.19410152055</v>
       </c>
     </row>
@@ -4769,7 +4766,7 @@
       <c r="E12" t="s">
         <v>141</v>
       </c>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="39" t="s">
         <v>133</v>
       </c>
       <c r="L12" s="17"/>
@@ -4791,15 +4788,15 @@
         <v>116</v>
       </c>
       <c r="L13" s="17"/>
-      <c r="M13" s="44">
+      <c r="M13" s="43">
         <f>$M$6*C46</f>
         <v>110916.81595518051</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="36">
         <f>$N$6*C46</f>
         <v>58233.653855551536</v>
       </c>
-      <c r="O13" s="45">
+      <c r="O13" s="44">
         <f>$O$6*C46</f>
         <v>36335.310466395342</v>
       </c>
@@ -4814,13 +4811,13 @@
       <c r="D14" s="19">
         <v>38377</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="41">
         <v>1734.9</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="46">
+      <c r="M14" s="45">
         <f>$M$6*D54</f>
         <v>44366.726382072207</v>
       </c>
@@ -4828,7 +4825,7 @@
         <f>$N$6*D54</f>
         <v>23293.461542220615</v>
       </c>
-      <c r="O14" s="47">
+      <c r="O14" s="46">
         <f>$O$6*D54</f>
         <v>14534.124186558138</v>
       </c>
@@ -4843,13 +4840,13 @@
       <c r="D15" s="33">
         <v>-0.65400000000000003</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <v>-0.26600000000000001</v>
       </c>
       <c r="L15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="46">
+      <c r="M15" s="45">
         <f t="shared" ref="M15:M18" si="0">$M$6*D55</f>
         <v>31056.708467450542</v>
       </c>
@@ -4857,7 +4854,7 @@
         <f t="shared" ref="N15:N18" si="1">$N$6*D55</f>
         <v>16305.42307955443</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="46">
         <f t="shared" ref="O15:O18" si="2">$O$6*D55</f>
         <v>10173.886930590697</v>
       </c>
@@ -4866,7 +4863,7 @@
       <c r="L16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="46">
+      <c r="M16" s="45">
         <f t="shared" si="0"/>
         <v>27729.203988795129</v>
       </c>
@@ -4874,7 +4871,7 @@
         <f t="shared" si="1"/>
         <v>14558.413463887884</v>
       </c>
-      <c r="O16" s="47">
+      <c r="O16" s="46">
         <f t="shared" si="2"/>
         <v>9083.8276165988354</v>
       </c>
@@ -4884,7 +4881,7 @@
       <c r="L17" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="M17" s="46">
+      <c r="M17" s="45">
         <f t="shared" si="0"/>
         <v>5545.8407977590259</v>
       </c>
@@ -4892,7 +4889,7 @@
         <f t="shared" si="1"/>
         <v>2911.6826927775769</v>
       </c>
-      <c r="O17" s="47">
+      <c r="O17" s="46">
         <f t="shared" si="2"/>
         <v>1816.7655233197672</v>
       </c>
@@ -4907,7 +4904,7 @@
       <c r="L18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="45">
         <f t="shared" si="0"/>
         <v>2218.3363191036105</v>
       </c>
@@ -4915,7 +4912,7 @@
         <f t="shared" si="1"/>
         <v>1164.6730771110308</v>
       </c>
-      <c r="O18" s="47">
+      <c r="O18" s="46">
         <f t="shared" si="2"/>
         <v>726.706209327907</v>
       </c>
@@ -4936,15 +4933,15 @@
         <v>117</v>
       </c>
       <c r="L19" s="17"/>
-      <c r="M19" s="48">
+      <c r="M19" s="47">
         <f>$M$6*C47</f>
         <v>98118.721806505841</v>
       </c>
-      <c r="N19" s="38">
+      <c r="N19" s="37">
         <f>$N$6*C47</f>
         <v>51514.386102987897</v>
       </c>
-      <c r="O19" s="49">
+      <c r="O19" s="48">
         <f>$O$6*C47</f>
         <v>32142.774643349727</v>
       </c>
@@ -4964,7 +4961,7 @@
       <c r="L20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="45">
         <f>$M$6*D61</f>
         <v>32379.178196146928</v>
       </c>
@@ -4972,7 +4969,7 @@
         <f>$N$6*D61</f>
         <v>16999.747413986006</v>
       </c>
-      <c r="O20" s="47">
+      <c r="O20" s="46">
         <f>$O$6*D61</f>
         <v>10607.115632305411</v>
       </c>
@@ -4992,7 +4989,7 @@
       <c r="L21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="M21" s="46">
+      <c r="M21" s="45">
         <f t="shared" ref="M21:M25" si="4">$M$6*D62</f>
         <v>21586.118797431282</v>
       </c>
@@ -5000,7 +4997,7 @@
         <f t="shared" ref="N21:N25" si="5">$N$6*D62</f>
         <v>11333.164942657337</v>
       </c>
-      <c r="O21" s="47">
+      <c r="O21" s="46">
         <f t="shared" ref="O21:O25" si="6">$O$6*D62</f>
         <v>7071.4104215369398</v>
       </c>
@@ -5019,7 +5016,7 @@
       <c r="L22" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="M22" s="46">
+      <c r="M22" s="45">
         <f t="shared" si="4"/>
         <v>18642.55714323611</v>
       </c>
@@ -5027,7 +5024,7 @@
         <f t="shared" si="5"/>
         <v>9787.733359567701</v>
       </c>
-      <c r="O22" s="47">
+      <c r="O22" s="46">
         <f t="shared" si="6"/>
         <v>6107.1271822364488</v>
       </c>
@@ -5046,7 +5043,7 @@
       <c r="L23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="46">
+      <c r="M23" s="45">
         <f t="shared" si="4"/>
         <v>11774.2466167807</v>
       </c>
@@ -5054,7 +5051,7 @@
         <f t="shared" si="5"/>
         <v>6181.7263323585476</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O23" s="46">
         <f t="shared" si="6"/>
         <v>3857.1329572019672</v>
       </c>
@@ -5073,7 +5070,7 @@
       <c r="L24" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="45">
         <f t="shared" si="4"/>
         <v>8830.6849625855248</v>
       </c>
@@ -5081,7 +5078,7 @@
         <f t="shared" si="5"/>
         <v>4636.2947492689109</v>
       </c>
-      <c r="O24" s="47">
+      <c r="O24" s="46">
         <f t="shared" si="6"/>
         <v>2892.8497179014753</v>
       </c>
@@ -5100,7 +5097,7 @@
       <c r="L25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M25" s="46">
+      <c r="M25" s="45">
         <f t="shared" si="4"/>
         <v>4905.9360903252918</v>
       </c>
@@ -5108,7 +5105,7 @@
         <f t="shared" si="5"/>
         <v>2575.719305149395</v>
       </c>
-      <c r="O25" s="47">
+      <c r="O25" s="46">
         <f t="shared" si="6"/>
         <v>1607.1387321674865</v>
       </c>
@@ -5128,15 +5125,15 @@
         <v>118</v>
       </c>
       <c r="L26" s="17"/>
-      <c r="M26" s="48">
+      <c r="M26" s="47">
         <f>$M$6*C48</f>
         <v>89586.659040722705</v>
       </c>
-      <c r="N26" s="38">
+      <c r="N26" s="37">
         <f>$N$6*C48</f>
         <v>47034.874267945466</v>
       </c>
-      <c r="O26" s="49">
+      <c r="O26" s="48">
         <f>$O$6*C48</f>
         <v>29347.750761319316</v>
       </c>
@@ -5146,15 +5143,15 @@
         <v>119</v>
       </c>
       <c r="L27" s="17"/>
-      <c r="M27" s="48">
+      <c r="M27" s="47">
         <f>$M$6*C49</f>
         <v>76788.564892048045</v>
       </c>
-      <c r="N27" s="38">
+      <c r="N27" s="37">
         <f t="shared" ref="N27:N29" si="7">$N$6*C49</f>
         <v>40315.606515381827</v>
       </c>
-      <c r="O27" s="49">
+      <c r="O27" s="48">
         <f t="shared" ref="O27:O29" si="8">$O$6*C49</f>
         <v>25155.214938273697</v>
       </c>
@@ -5174,15 +5171,15 @@
         <v>121</v>
       </c>
       <c r="L28" s="17"/>
-      <c r="M28" s="48">
+      <c r="M28" s="47">
         <f>$M$6*C50</f>
         <v>38394.282446024023</v>
       </c>
-      <c r="N28" s="38">
+      <c r="N28" s="37">
         <f t="shared" si="7"/>
         <v>20157.803257690914</v>
       </c>
-      <c r="O28" s="49">
+      <c r="O28" s="48">
         <f t="shared" si="8"/>
         <v>12577.607469136849</v>
       </c>
@@ -5203,15 +5200,15 @@
         <v>122</v>
       </c>
       <c r="L29" s="17"/>
-      <c r="M29" s="50">
+      <c r="M29" s="49">
         <f>$M$6*C51</f>
         <v>12798.094148674672</v>
       </c>
-      <c r="N29" s="39">
+      <c r="N29" s="38">
         <f t="shared" si="7"/>
         <v>6719.2677525636382</v>
       </c>
-      <c r="O29" s="51">
+      <c r="O29" s="50">
         <f t="shared" si="8"/>
         <v>4192.5358230456168</v>
       </c>
@@ -5242,7 +5239,7 @@
         <v>1.1404204680682268</v>
       </c>
       <c r="E31" s="15"/>
-      <c r="K31" s="40" t="s">
+      <c r="K31" s="39" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5286,7 +5283,7 @@
         <f>$N$6*C70</f>
         <v>47034.874267945466</v>
       </c>
-      <c r="O33" s="42">
+      <c r="O33" s="41">
         <f>$O$6*C70</f>
         <v>29347.750761319316</v>
       </c>
@@ -5306,7 +5303,7 @@
       <c r="K34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="46">
+      <c r="M34" s="45">
         <f t="shared" ref="M34:M41" si="10">$M$6*C71</f>
         <v>85320.627657831166</v>
       </c>
@@ -5314,7 +5311,7 @@
         <f t="shared" ref="N34:N41" si="11">$N$6*C71</f>
         <v>44795.118350424258</v>
       </c>
-      <c r="O34" s="47">
+      <c r="O34" s="46">
         <f t="shared" ref="O34:O41" si="12">$O$6*C71</f>
         <v>27950.238820304112</v>
       </c>
@@ -5334,7 +5331,7 @@
       <c r="K35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M35" s="46">
+      <c r="M35" s="45">
         <f t="shared" si="10"/>
         <v>72522.533509156492</v>
       </c>
@@ -5342,7 +5339,7 @@
         <f t="shared" si="11"/>
         <v>38075.850597860619</v>
       </c>
-      <c r="O35" s="47">
+      <c r="O35" s="46">
         <f t="shared" si="12"/>
         <v>23757.702997258497</v>
       </c>
@@ -5362,7 +5359,7 @@
       <c r="K36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M36" s="46">
+      <c r="M36" s="45">
         <f t="shared" si="10"/>
         <v>38394.282446024023</v>
       </c>
@@ -5370,7 +5367,7 @@
         <f t="shared" si="11"/>
         <v>20157.803257690914</v>
       </c>
-      <c r="O36" s="47">
+      <c r="O36" s="46">
         <f t="shared" si="12"/>
         <v>12577.607469136849</v>
       </c>
@@ -5390,7 +5387,7 @@
       <c r="K37" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M37" s="46">
+      <c r="M37" s="45">
         <f t="shared" si="10"/>
         <v>34128.251063132462</v>
       </c>
@@ -5398,7 +5395,7 @@
         <f t="shared" si="11"/>
         <v>17918.047340169702</v>
       </c>
-      <c r="O37" s="47">
+      <c r="O37" s="46">
         <f t="shared" si="12"/>
         <v>11180.095528121645</v>
       </c>
@@ -5418,7 +5415,7 @@
       <c r="K38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M38" s="46">
+      <c r="M38" s="45">
         <f t="shared" si="10"/>
         <v>29862.219680240909</v>
       </c>
@@ -5426,7 +5423,7 @@
         <f t="shared" si="11"/>
         <v>15678.291422648492</v>
       </c>
-      <c r="O38" s="47">
+      <c r="O38" s="46">
         <f t="shared" si="12"/>
         <v>9782.5835871064392</v>
       </c>
@@ -5446,7 +5443,7 @@
       <c r="K39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M39" s="46">
+      <c r="M39" s="45">
         <f t="shared" si="10"/>
         <v>25596.188297349345</v>
       </c>
@@ -5454,7 +5451,7 @@
         <f t="shared" si="11"/>
         <v>13438.535505127276</v>
       </c>
-      <c r="O39" s="47">
+      <c r="O39" s="46">
         <f t="shared" si="12"/>
         <v>8385.0716460912336</v>
       </c>
@@ -5474,7 +5471,7 @@
       <c r="K40" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="46">
+      <c r="M40" s="45">
         <f t="shared" si="10"/>
         <v>25596.188297349345</v>
       </c>
@@ -5482,7 +5479,7 @@
         <f t="shared" si="11"/>
         <v>13438.535505127276</v>
       </c>
-      <c r="O40" s="47">
+      <c r="O40" s="46">
         <f t="shared" si="12"/>
         <v>8385.0716460912336</v>
       </c>
@@ -5510,7 +5507,7 @@
         <f t="shared" si="11"/>
         <v>11198.779587606065</v>
       </c>
-      <c r="O41" s="43">
+      <c r="O41" s="42">
         <f t="shared" si="12"/>
         <v>6987.559705076028</v>
       </c>
@@ -5898,8 +5895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,27 +5914,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="41"/>
+      <c r="A1" s="40"/>
       <c r="B1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
       <c r="G1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="9" t="s">
         <v>102</v>
       </c>
       <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="39" t="s">
         <v>135</v>
       </c>
       <c r="M2" s="15" t="s">
@@ -5960,8 +5957,8 @@
       <c r="G3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="36">
-        <v>0.2</v>
+      <c r="H3" s="13">
+        <v>10024</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>143</v>
@@ -5990,6 +5987,7 @@
         <f>VLOOKUP(B4,B19:D26,3,0)</f>
         <v>0.48</v>
       </c>
+      <c r="H4" s="52"/>
       <c r="K4" s="15" t="s">
         <v>108</v>
       </c>
@@ -6023,16 +6021,16 @@
         <v>132</v>
       </c>
       <c r="M6" s="13">
-        <f>H3*M4</f>
-        <v>670679.61521042546</v>
+        <f>H3*M3</f>
+        <v>670639.47318290046</v>
       </c>
       <c r="N6" s="13">
-        <f>H3*N4</f>
-        <v>148382.24166681952</v>
+        <f>H3*N3</f>
+        <v>148373.3605797936</v>
       </c>
       <c r="O6" s="13">
-        <f>H3*O4</f>
-        <v>446889.06789390167</v>
+        <f>H3*O3</f>
+        <v>446862.32034878898</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -6053,7 +6051,7 @@
       <c r="E12" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="39" t="s">
         <v>133</v>
       </c>
       <c r="L12" s="17"/>
@@ -6075,17 +6073,17 @@
         <v>116</v>
       </c>
       <c r="L13" s="17"/>
-      <c r="M13" s="44">
+      <c r="M13" s="43">
         <f>$M$6*C46</f>
-        <v>174376.69995471064</v>
-      </c>
-      <c r="N13" s="37">
+        <v>174366.26302755412</v>
+      </c>
+      <c r="N13" s="36">
         <f>$N$6*C46</f>
-        <v>38579.382833373078</v>
-      </c>
-      <c r="O13" s="45">
+        <v>38577.073750746342</v>
+      </c>
+      <c r="O13" s="44">
         <f>$O$6*C46</f>
-        <v>116191.15765241443</v>
+        <v>116184.20329068514</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -6098,23 +6096,23 @@
       <c r="D14" s="19">
         <v>38377</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="41">
         <v>1734.9</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="46">
+      <c r="M14" s="45">
         <f>$M$6*D54</f>
-        <v>69750.679981884256</v>
+        <v>69746.505211021649</v>
       </c>
       <c r="N14" s="32">
         <f>$N$6*D54</f>
-        <v>15431.753133349232</v>
-      </c>
-      <c r="O14" s="47">
+        <v>15430.829500298536</v>
+      </c>
+      <c r="O14" s="46">
         <f>$O$6*D54</f>
-        <v>46476.463060965776</v>
+        <v>46473.681316274058</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6127,40 +6125,40 @@
       <c r="D15" s="33">
         <v>-0.65400000000000003</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <v>-0.26600000000000001</v>
       </c>
       <c r="L15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="46">
-        <f t="shared" ref="M15:M18" si="0">$M$6*D55</f>
-        <v>48825.475987318976</v>
+      <c r="M15" s="45">
+        <f>$M$6*D55</f>
+        <v>48822.553647715155</v>
       </c>
       <c r="N15" s="32">
-        <f t="shared" ref="N15:N18" si="1">$N$6*D55</f>
-        <v>10802.227193344461</v>
-      </c>
-      <c r="O15" s="47">
-        <f t="shared" ref="O15:O18" si="2">$O$6*D55</f>
-        <v>32533.524142676044</v>
+        <f>$N$6*D55</f>
+        <v>10801.580650208974</v>
+      </c>
+      <c r="O15" s="46">
+        <f>$O$6*D55</f>
+        <v>32531.576921391839</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="46">
-        <f t="shared" si="0"/>
-        <v>43594.17498867766</v>
+      <c r="M16" s="45">
+        <f>$M$6*D56</f>
+        <v>43591.565756888529</v>
       </c>
       <c r="N16" s="32">
-        <f t="shared" si="1"/>
-        <v>9644.8457083432695</v>
-      </c>
-      <c r="O16" s="47">
-        <f t="shared" si="2"/>
-        <v>29047.789413103608</v>
+        <f>$N$6*D56</f>
+        <v>9644.2684376865855</v>
+      </c>
+      <c r="O16" s="46">
+        <f>$O$6*D56</f>
+        <v>29046.050822671285</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -6168,17 +6166,17 @@
       <c r="L17" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="M17" s="46">
-        <f t="shared" si="0"/>
-        <v>8718.8349977355319</v>
+      <c r="M17" s="45">
+        <f>$M$6*D57</f>
+        <v>8718.3131513777062</v>
       </c>
       <c r="N17" s="32">
-        <f t="shared" si="1"/>
-        <v>1928.9691416686539</v>
-      </c>
-      <c r="O17" s="47">
-        <f t="shared" si="2"/>
-        <v>5809.557882620722</v>
+        <f>$N$6*D57</f>
+        <v>1928.853687537317</v>
+      </c>
+      <c r="O17" s="46">
+        <f>$O$6*D57</f>
+        <v>5809.2101645342573</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6190,17 +6188,17 @@
       <c r="L18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="46">
-        <f t="shared" si="0"/>
-        <v>3487.533999094213</v>
+      <c r="M18" s="45">
+        <f>$M$6*D58</f>
+        <v>3487.3252605510829</v>
       </c>
       <c r="N18" s="32">
-        <f t="shared" si="1"/>
-        <v>771.5876566674616</v>
-      </c>
-      <c r="O18" s="47">
-        <f t="shared" si="2"/>
-        <v>2323.823153048289</v>
+        <f>$N$6*D58</f>
+        <v>771.54147501492685</v>
+      </c>
+      <c r="O18" s="46">
+        <f>$O$6*D58</f>
+        <v>2323.684065813703</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -6219,17 +6217,17 @@
         <v>117</v>
       </c>
       <c r="L19" s="17"/>
-      <c r="M19" s="48">
+      <c r="M19" s="47">
         <f>$M$6*C47</f>
-        <v>154256.31149839787</v>
-      </c>
-      <c r="N19" s="38">
+        <v>154247.07883206711</v>
+      </c>
+      <c r="N19" s="37">
         <f>$N$6*C47</f>
-        <v>34127.915583368493</v>
-      </c>
-      <c r="O19" s="49">
+        <v>34125.872933352533</v>
+      </c>
+      <c r="O19" s="48">
         <f>$O$6*C47</f>
-        <v>102784.48561559738</v>
+        <v>102778.33368022148</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -6240,24 +6238,24 @@
         <v>0.3</v>
       </c>
       <c r="D20" s="27">
-        <f t="shared" ref="D20:D26" si="3">1-C20</f>
+        <f t="shared" ref="D20:D26" si="0">1-C20</f>
         <v>0.7</v>
       </c>
       <c r="I20" s="16"/>
       <c r="L20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="45">
         <f>$M$6*D61</f>
-        <v>50904.582794471302</v>
+        <v>50901.536014582154</v>
       </c>
       <c r="N20" s="32">
         <f>$N$6*D61</f>
-        <v>11262.212142511604</v>
-      </c>
-      <c r="O20" s="47">
+        <v>11261.538068006335</v>
+      </c>
+      <c r="O20" s="46">
         <f>$O$6*D61</f>
-        <v>33918.880253147137</v>
+        <v>33916.850114473091</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -6268,24 +6266,24 @@
         <v>0.36</v>
       </c>
       <c r="D21" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
       <c r="I21" s="16"/>
       <c r="L21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="M21" s="46">
-        <f t="shared" ref="M21:M25" si="4">$M$6*D62</f>
-        <v>33936.388529647527</v>
+      <c r="M21" s="45">
+        <f>$M$6*D62</f>
+        <v>33934.357343054762</v>
       </c>
       <c r="N21" s="32">
-        <f t="shared" ref="N21:N25" si="5">$N$6*D62</f>
-        <v>7508.1414283410677</v>
-      </c>
-      <c r="O21" s="47">
-        <f t="shared" ref="O21:O25" si="6">$O$6*D62</f>
-        <v>22612.586835431423</v>
+        <f>$N$6*D62</f>
+        <v>7507.692045337556</v>
+      </c>
+      <c r="O21" s="46">
+        <f>$O$6*D62</f>
+        <v>22611.233409648721</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -6296,23 +6294,23 @@
         <v>0.45</v>
       </c>
       <c r="D22" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L22" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="M22" s="46">
-        <f t="shared" si="4"/>
-        <v>29308.699184695593</v>
+      <c r="M22" s="45">
+        <f>$M$6*D63</f>
+        <v>29306.944978092753</v>
       </c>
       <c r="N22" s="32">
-        <f t="shared" si="5"/>
-        <v>6484.3039608400131</v>
-      </c>
-      <c r="O22" s="47">
-        <f t="shared" si="6"/>
-        <v>19529.052266963503</v>
+        <f>$N$6*D63</f>
+        <v>6483.9158573369805</v>
+      </c>
+      <c r="O22" s="46">
+        <f>$O$6*D63</f>
+        <v>19527.88339924208</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -6323,23 +6321,23 @@
         <v>0.52</v>
       </c>
       <c r="D23" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="46">
-        <f t="shared" si="4"/>
-        <v>18510.757379807743</v>
+      <c r="M23" s="45">
+        <f>$M$6*D64</f>
+        <v>18509.649459848053</v>
       </c>
       <c r="N23" s="32">
-        <f t="shared" si="5"/>
-        <v>4095.3498700042187</v>
-      </c>
-      <c r="O23" s="47">
-        <f t="shared" si="6"/>
-        <v>12334.138273871686</v>
+        <f>$N$6*D64</f>
+        <v>4095.1047520023035</v>
+      </c>
+      <c r="O23" s="46">
+        <f>$O$6*D64</f>
+        <v>12333.400041626575</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -6350,23 +6348,23 @@
         <v>0.61</v>
       </c>
       <c r="D24" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="L24" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="46">
-        <f t="shared" si="4"/>
-        <v>13883.068034855807</v>
+      <c r="M24" s="45">
+        <f>$M$6*D65</f>
+        <v>13882.237094886039</v>
       </c>
       <c r="N24" s="32">
-        <f t="shared" si="5"/>
-        <v>3071.5124025031641</v>
-      </c>
-      <c r="O24" s="47">
-        <f t="shared" si="6"/>
-        <v>9250.6037054037643</v>
+        <f>$N$6*D65</f>
+        <v>3071.3285640017275</v>
+      </c>
+      <c r="O24" s="46">
+        <f>$O$6*D65</f>
+        <v>9250.050031219931</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -6377,23 +6375,23 @@
         <v>0.64</v>
       </c>
       <c r="D25" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
       <c r="L25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M25" s="46">
-        <f t="shared" si="4"/>
-        <v>7712.8155749198941</v>
+      <c r="M25" s="45">
+        <f>$M$6*D66</f>
+        <v>7712.3539416033564</v>
       </c>
       <c r="N25" s="32">
-        <f t="shared" si="5"/>
-        <v>1706.3957791684247</v>
-      </c>
-      <c r="O25" s="47">
-        <f t="shared" si="6"/>
-        <v>5139.2242807798702</v>
+        <f>$N$6*D66</f>
+        <v>1706.2936466676267</v>
+      </c>
+      <c r="O25" s="46">
+        <f>$O$6*D66</f>
+        <v>5138.9166840110738</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6404,24 +6402,24 @@
         <v>0</v>
       </c>
       <c r="D26" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K26" s="17" t="s">
         <v>118</v>
       </c>
       <c r="L26" s="17"/>
-      <c r="M26" s="48">
+      <c r="M26" s="47">
         <f>$M$6*C48</f>
-        <v>140842.71919418935</v>
-      </c>
-      <c r="N26" s="38">
+        <v>140834.28936840908</v>
+      </c>
+      <c r="N26" s="37">
         <f>$N$6*C48</f>
-        <v>31160.270750032098</v>
-      </c>
-      <c r="O26" s="49">
+        <v>31158.405721756655</v>
+      </c>
+      <c r="O26" s="48">
         <f>$O$6*C48</f>
-        <v>93846.70425771935</v>
+        <v>93841.087273245677</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -6429,17 +6427,17 @@
         <v>119</v>
       </c>
       <c r="L27" s="17"/>
-      <c r="M27" s="48">
+      <c r="M27" s="47">
         <f>$M$6*C49</f>
-        <v>120722.33073787657</v>
-      </c>
-      <c r="N27" s="38">
-        <f t="shared" ref="N27:N29" si="7">$N$6*C49</f>
-        <v>26708.803500027512</v>
-      </c>
-      <c r="O27" s="49">
-        <f t="shared" ref="O27:O29" si="8">$O$6*C49</f>
-        <v>80440.0322209023</v>
+        <v>120715.10517292208</v>
+      </c>
+      <c r="N27" s="37">
+        <f>$N$6*C49</f>
+        <v>26707.204904362847</v>
+      </c>
+      <c r="O27" s="48">
+        <f>$O$6*C49</f>
+        <v>80435.217662782015</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6456,17 +6454,17 @@
         <v>121</v>
       </c>
       <c r="L28" s="17"/>
-      <c r="M28" s="48">
+      <c r="M28" s="47">
         <f>$M$6*C50</f>
-        <v>60361.165368938287</v>
-      </c>
-      <c r="N28" s="38">
-        <f t="shared" si="7"/>
-        <v>13354.401750013756</v>
-      </c>
-      <c r="O28" s="49">
-        <f t="shared" si="8"/>
-        <v>40220.01611045115</v>
+        <v>60357.552586461039</v>
+      </c>
+      <c r="N28" s="37">
+        <f>$N$6*C50</f>
+        <v>13353.602452181423</v>
+      </c>
+      <c r="O28" s="48">
+        <f>$O$6*C50</f>
+        <v>40217.608831391008</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6477,24 +6475,24 @@
         <v>7.45</v>
       </c>
       <c r="D29" s="29">
-        <f t="shared" ref="D29:D42" si="9">(C29/$E$28)</f>
+        <f t="shared" ref="D29:D42" si="1">(C29/$E$28)</f>
         <v>1.5391544360703424</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>122</v>
       </c>
       <c r="L29" s="17"/>
-      <c r="M29" s="50">
+      <c r="M29" s="49">
         <f>$M$6*C51</f>
-        <v>20120.388456312761</v>
-      </c>
-      <c r="N29" s="39">
-        <f t="shared" si="7"/>
-        <v>4451.4672500045854</v>
-      </c>
-      <c r="O29" s="51">
-        <f t="shared" si="8"/>
-        <v>13406.67203681705</v>
+        <v>20119.184195487014</v>
+      </c>
+      <c r="N29" s="38">
+        <f>$N$6*C51</f>
+        <v>4451.2008173938075</v>
+      </c>
+      <c r="O29" s="50">
+        <f>$O$6*C51</f>
+        <v>13405.869610463669</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -6505,7 +6503,7 @@
         <v>6.51</v>
       </c>
       <c r="D30" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>1.3449523998413326</v>
       </c>
       <c r="M30" s="17"/>
@@ -6518,10 +6516,10 @@
         <v>5.52</v>
       </c>
       <c r="D31" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>1.1404204680682268</v>
       </c>
-      <c r="K31" s="40" t="s">
+      <c r="K31" s="39" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6533,7 +6531,7 @@
         <v>5.26</v>
       </c>
       <c r="D32" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>1.0867050112389263</v>
       </c>
       <c r="K32" s="17" t="s">
@@ -6549,7 +6547,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="D33" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.95241636916567507</v>
       </c>
       <c r="K33" s="15" t="s">
@@ -6557,15 +6555,15 @@
       </c>
       <c r="M33" s="21">
         <f>$M$6*C70</f>
-        <v>140842.71919418935</v>
+        <v>140834.28936840908</v>
       </c>
       <c r="N33" s="19">
         <f>$N$6*C70</f>
-        <v>31160.270750032098</v>
-      </c>
-      <c r="O33" s="42">
+        <v>31158.405721756655</v>
+      </c>
+      <c r="O33" s="41">
         <f>$O$6*C70</f>
-        <v>93846.70425771935</v>
+        <v>93841.087273245677</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -6576,23 +6574,23 @@
         <v>4.57</v>
       </c>
       <c r="D34" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.94415245273039805</v>
       </c>
       <c r="K34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="46">
-        <f t="shared" ref="M34:M41" si="10">$M$6*C71</f>
-        <v>134135.92304208511</v>
+      <c r="M34" s="45">
+        <f>$M$6*C71</f>
+        <v>134127.89463658011</v>
       </c>
       <c r="N34" s="32">
-        <f t="shared" ref="N34:N41" si="11">$N$6*C71</f>
-        <v>29676.448333363907</v>
-      </c>
-      <c r="O34" s="47">
-        <f t="shared" ref="O34:O41" si="12">$O$6*C71</f>
-        <v>89377.813578780333</v>
+        <f>$N$6*C71</f>
+        <v>29674.672115958721</v>
+      </c>
+      <c r="O34" s="46">
+        <f>$O$6*C71</f>
+        <v>89372.4640697578</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -6603,23 +6601,23 @@
         <v>4.55</v>
       </c>
       <c r="D35" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.94002049451275937</v>
       </c>
       <c r="K35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M35" s="46">
-        <f t="shared" si="10"/>
-        <v>114015.53458577233</v>
+      <c r="M35" s="45">
+        <f>$M$6*C72</f>
+        <v>114008.71044109309</v>
       </c>
       <c r="N35" s="32">
-        <f t="shared" si="11"/>
-        <v>25224.981083359322</v>
-      </c>
-      <c r="O35" s="47">
-        <f t="shared" si="12"/>
-        <v>75971.141541963283</v>
+        <f>$N$6*C72</f>
+        <v>25223.471298564913</v>
+      </c>
+      <c r="O35" s="46">
+        <f>$O$6*C72</f>
+        <v>75966.594459294138</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -6630,23 +6628,23 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="D36" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.88217307946582035</v>
       </c>
       <c r="K36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M36" s="46">
-        <f t="shared" si="10"/>
-        <v>60361.165368938287</v>
+      <c r="M36" s="45">
+        <f>$M$6*C73</f>
+        <v>60357.552586461039</v>
       </c>
       <c r="N36" s="32">
-        <f t="shared" si="11"/>
-        <v>13354.401750013756</v>
-      </c>
-      <c r="O36" s="47">
-        <f t="shared" si="12"/>
-        <v>40220.01611045115</v>
+        <f>$N$6*C73</f>
+        <v>13353.602452181423</v>
+      </c>
+      <c r="O36" s="46">
+        <f>$O$6*C73</f>
+        <v>40217.608831391008</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -6657,23 +6655,23 @@
         <v>3.78</v>
       </c>
       <c r="D37" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.78094010313367701</v>
       </c>
       <c r="K37" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M37" s="46">
-        <f t="shared" si="10"/>
-        <v>53654.369216834035</v>
+      <c r="M37" s="45">
+        <f>$M$6*C74</f>
+        <v>53651.157854632038</v>
       </c>
       <c r="N37" s="32">
-        <f t="shared" si="11"/>
-        <v>11870.579333345562</v>
-      </c>
-      <c r="O37" s="47">
-        <f t="shared" si="12"/>
-        <v>35751.125431512133</v>
+        <f>$N$6*C74</f>
+        <v>11869.868846383488</v>
+      </c>
+      <c r="O37" s="46">
+        <f>$O$6*C74</f>
+        <v>35748.985627903123</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -6684,23 +6682,23 @@
         <v>3.47</v>
       </c>
       <c r="D38" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.71689475076028031</v>
       </c>
       <c r="K38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M38" s="46">
-        <f t="shared" si="10"/>
-        <v>46947.57306472979</v>
+      <c r="M38" s="45">
+        <f>$M$6*C75</f>
+        <v>46944.763122803037</v>
       </c>
       <c r="N38" s="32">
-        <f t="shared" si="11"/>
-        <v>10386.756916677368</v>
-      </c>
-      <c r="O38" s="47">
-        <f t="shared" si="12"/>
-        <v>31282.23475257312</v>
+        <f>$N$6*C75</f>
+        <v>10386.135240585554</v>
+      </c>
+      <c r="O38" s="46">
+        <f>$O$6*C75</f>
+        <v>31280.362424415231</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -6711,23 +6709,23 @@
         <v>3.39</v>
       </c>
       <c r="D39" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.70036691788972627</v>
       </c>
       <c r="K39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M39" s="46">
-        <f t="shared" si="10"/>
-        <v>40240.776912625523</v>
+      <c r="M39" s="45">
+        <f>$M$6*C76</f>
+        <v>40238.368390974028</v>
       </c>
       <c r="N39" s="32">
-        <f t="shared" si="11"/>
-        <v>8902.9345000091707</v>
-      </c>
-      <c r="O39" s="47">
-        <f t="shared" si="12"/>
-        <v>26813.3440736341</v>
+        <f>$N$6*C76</f>
+        <v>8902.401634787615</v>
+      </c>
+      <c r="O39" s="46">
+        <f>$O$6*C76</f>
+        <v>26811.739220927338</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -6738,23 +6736,23 @@
         <v>3.04</v>
       </c>
       <c r="D40" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.62805764908105244</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="46">
-        <f t="shared" si="10"/>
-        <v>40240.776912625523</v>
+      <c r="M40" s="45">
+        <f>$M$6*C77</f>
+        <v>40238.368390974028</v>
       </c>
       <c r="N40" s="32">
-        <f t="shared" si="11"/>
-        <v>8902.9345000091707</v>
-      </c>
-      <c r="O40" s="47">
-        <f t="shared" si="12"/>
-        <v>26813.3440736341</v>
+        <f>$N$6*C77</f>
+        <v>8902.401634787615</v>
+      </c>
+      <c r="O40" s="46">
+        <f>$O$6*C77</f>
+        <v>26811.739220927338</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6765,23 +6763,23 @@
         <v>2.91</v>
       </c>
       <c r="D41" s="30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.60119992066640227</v>
       </c>
       <c r="K41" s="15" t="s">
         <v>18</v>
       </c>
       <c r="M41" s="22">
-        <f t="shared" si="10"/>
-        <v>33533.980760521277</v>
+        <f>$M$6*C78</f>
+        <v>33531.973659145027</v>
       </c>
       <c r="N41" s="33">
-        <f t="shared" si="11"/>
-        <v>7419.1120833409768</v>
-      </c>
-      <c r="O41" s="43">
-        <f t="shared" si="12"/>
-        <v>22344.453394695083</v>
+        <f>$N$6*C78</f>
+        <v>7418.6680289896804</v>
+      </c>
+      <c r="O41" s="42">
+        <f>$O$6*C78</f>
+        <v>22343.11601743945</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6792,7 +6790,7 @@
         <v>1.91</v>
       </c>
       <c r="D42" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.39460200978447701</v>
       </c>
     </row>
@@ -6885,7 +6883,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D55" s="27">
-        <f t="shared" ref="D55:D58" si="13">C55*$C$46</f>
+        <f t="shared" ref="D55:D58" si="2">C55*$C$46</f>
         <v>7.2800000000000004E-2</v>
       </c>
     </row>
@@ -6897,7 +6895,7 @@
         <v>0.25</v>
       </c>
       <c r="D56" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
@@ -6909,7 +6907,7 @@
         <v>0.05</v>
       </c>
       <c r="D57" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>1.3000000000000001E-2</v>
       </c>
     </row>
@@ -6921,7 +6919,7 @@
         <v>0.02</v>
       </c>
       <c r="D58" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>5.2000000000000006E-3</v>
       </c>
     </row>
@@ -6953,7 +6951,7 @@
         <v>0.22</v>
       </c>
       <c r="D62" s="27">
-        <f t="shared" ref="D62:D66" si="14">C62*$C$47</f>
+        <f t="shared" ref="D62:D66" si="3">C62*$C$47</f>
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
@@ -6965,7 +6963,7 @@
         <v>0.19</v>
       </c>
       <c r="D63" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
@@ -6977,7 +6975,7 @@
         <v>0.12</v>
       </c>
       <c r="D64" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>2.76E-2</v>
       </c>
     </row>
@@ -6989,7 +6987,7 @@
         <v>0.09</v>
       </c>
       <c r="D65" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>2.07E-2</v>
       </c>
     </row>
@@ -7001,7 +6999,7 @@
         <v>0.05</v>
       </c>
       <c r="D66" s="28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>1.1500000000000002E-2</v>
       </c>
     </row>
@@ -7116,7 +7114,7 @@
       <c r="C88" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>$B$29:$B$42</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update Daten Analyse Viren
</commit_message>
<xml_diff>
--- a/documentation/DatenAnalyse Viren.xlsx
+++ b/documentation/DatenAnalyse Viren.xlsx
@@ -1051,11 +1051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51779776"/>
-        <c:axId val="51780352"/>
+        <c:axId val="78656576"/>
+        <c:axId val="78657152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51779776"/>
+        <c:axId val="78656576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000"/>
@@ -1066,12 +1066,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51780352"/>
+        <c:crossAx val="78657152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51780352"/>
+        <c:axId val="78657152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,13 +1082,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51779776"/>
+        <c:crossAx val="78656576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1118,6 +1119,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1435,11 +1437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44795008"/>
-        <c:axId val="44795584"/>
+        <c:axId val="131497984"/>
+        <c:axId val="131498560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44795008"/>
+        <c:axId val="131497984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,12 +1451,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44795584"/>
+        <c:crossAx val="131498560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44795584"/>
+        <c:axId val="131498560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,13 +1467,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44795008"/>
+        <c:crossAx val="131497984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1501,6 +1504,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1690,11 +1694,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45006336"/>
-        <c:axId val="44797312"/>
+        <c:axId val="131545088"/>
+        <c:axId val="131500288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45006336"/>
+        <c:axId val="131545088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44797312"/>
+        <c:crossAx val="131500288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1711,7 +1715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44797312"/>
+        <c:axId val="131500288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,13 +1726,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45006336"/>
+        <c:crossAx val="131545088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2242,11 +2247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44799040"/>
-        <c:axId val="44799616"/>
+        <c:axId val="131502016"/>
+        <c:axId val="131502592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44799040"/>
+        <c:axId val="131502016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000"/>
@@ -2257,12 +2262,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44799616"/>
+        <c:crossAx val="131502592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44799616"/>
+        <c:axId val="131502592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,7 +2278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44799040"/>
+        <c:crossAx val="131502016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3296,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4615,7 +4620,7 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4685,7 +4690,7 @@
       </c>
       <c r="N3" s="19">
         <f>D14*POWER(C3,D15)*C4*C5</f>
-        <v>516.66803172346317</v>
+        <v>5166.7476320366904</v>
       </c>
       <c r="O3" s="19">
         <f>E14*POWER(C3,E15)*C4*C5</f>
@@ -4712,7 +4717,7 @@
       </c>
       <c r="N4" s="13">
         <f>N3*C3</f>
-        <v>447951.18350424257</v>
+        <v>4479570.1969758105</v>
       </c>
       <c r="O4" s="13">
         <f>O3*C3</f>
@@ -4741,7 +4746,7 @@
       </c>
       <c r="N6" s="13">
         <f>H3*N3</f>
-        <v>223975.59175212128</v>
+        <v>2239785.0984879052</v>
       </c>
       <c r="O6" s="13">
         <f>H3*O3</f>
@@ -4794,7 +4799,7 @@
       </c>
       <c r="N13" s="36">
         <f>$N$6*C46</f>
-        <v>58233.653855551536</v>
+        <v>582344.12560685538</v>
       </c>
       <c r="O13" s="44">
         <f>$O$6*C46</f>
@@ -4809,7 +4814,7 @@
         <v>17302</v>
       </c>
       <c r="D14" s="19">
-        <v>38377</v>
+        <v>383775</v>
       </c>
       <c r="E14" s="41">
         <v>1734.9</v>
@@ -4823,7 +4828,7 @@
       </c>
       <c r="N14" s="32">
         <f>$N$6*D54</f>
-        <v>23293.461542220615</v>
+        <v>232937.65024274215</v>
       </c>
       <c r="O14" s="46">
         <f>$O$6*D54</f>
@@ -4852,7 +4857,7 @@
       </c>
       <c r="N15" s="32">
         <f t="shared" ref="N15:N18" si="1">$N$6*D55</f>
-        <v>16305.42307955443</v>
+        <v>163056.35516991949</v>
       </c>
       <c r="O15" s="46">
         <f t="shared" ref="O15:O18" si="2">$O$6*D55</f>
@@ -4869,7 +4874,7 @@
       </c>
       <c r="N16" s="32">
         <f t="shared" si="1"/>
-        <v>14558.413463887884</v>
+        <v>145586.03140171384</v>
       </c>
       <c r="O16" s="46">
         <f t="shared" si="2"/>
@@ -4887,7 +4892,7 @@
       </c>
       <c r="N17" s="32">
         <f t="shared" si="1"/>
-        <v>2911.6826927775769</v>
+        <v>29117.206280342769</v>
       </c>
       <c r="O17" s="46">
         <f t="shared" si="2"/>
@@ -4910,7 +4915,7 @@
       </c>
       <c r="N18" s="32">
         <f t="shared" si="1"/>
-        <v>1164.6730771110308</v>
+        <v>11646.882512137108</v>
       </c>
       <c r="O18" s="46">
         <f t="shared" si="2"/>
@@ -4939,7 +4944,7 @@
       </c>
       <c r="N19" s="37">
         <f>$N$6*C47</f>
-        <v>51514.386102987897</v>
+        <v>515150.57265221822</v>
       </c>
       <c r="O19" s="48">
         <f>$O$6*C47</f>
@@ -4967,7 +4972,7 @@
       </c>
       <c r="N20" s="32">
         <f>$N$6*D61</f>
-        <v>16999.747413986006</v>
+        <v>169999.68897523201</v>
       </c>
       <c r="O20" s="46">
         <f>$O$6*D61</f>
@@ -4995,7 +5000,7 @@
       </c>
       <c r="N21" s="32">
         <f t="shared" ref="N21:N25" si="5">$N$6*D62</f>
-        <v>11333.164942657337</v>
+        <v>113333.125983488</v>
       </c>
       <c r="O21" s="46">
         <f t="shared" ref="O21:O25" si="6">$O$6*D62</f>
@@ -5022,7 +5027,7 @@
       </c>
       <c r="N22" s="32">
         <f t="shared" si="5"/>
-        <v>9787.733359567701</v>
+        <v>97878.608803921466</v>
       </c>
       <c r="O22" s="46">
         <f t="shared" si="6"/>
@@ -5049,7 +5054,7 @@
       </c>
       <c r="N23" s="32">
         <f t="shared" si="5"/>
-        <v>6181.7263323585476</v>
+        <v>61818.068718266186</v>
       </c>
       <c r="O23" s="46">
         <f t="shared" si="6"/>
@@ -5076,7 +5081,7 @@
       </c>
       <c r="N24" s="32">
         <f t="shared" si="5"/>
-        <v>4636.2947492689109</v>
+        <v>46363.551538699634</v>
       </c>
       <c r="O24" s="46">
         <f t="shared" si="6"/>
@@ -5103,7 +5108,7 @@
       </c>
       <c r="N25" s="32">
         <f t="shared" si="5"/>
-        <v>2575.719305149395</v>
+        <v>25757.528632610913</v>
       </c>
       <c r="O25" s="46">
         <f t="shared" si="6"/>
@@ -5131,7 +5136,7 @@
       </c>
       <c r="N26" s="37">
         <f>$N$6*C48</f>
-        <v>47034.874267945466</v>
+        <v>470354.87068246008</v>
       </c>
       <c r="O26" s="48">
         <f>$O$6*C48</f>
@@ -5149,7 +5154,7 @@
       </c>
       <c r="N27" s="37">
         <f t="shared" ref="N27:N29" si="7">$N$6*C49</f>
-        <v>40315.606515381827</v>
+        <v>403161.31772782293</v>
       </c>
       <c r="O27" s="48">
         <f t="shared" ref="O27:O29" si="8">$O$6*C49</f>
@@ -5177,7 +5182,7 @@
       </c>
       <c r="N28" s="37">
         <f t="shared" si="7"/>
-        <v>20157.803257690914</v>
+        <v>201580.65886391146</v>
       </c>
       <c r="O28" s="48">
         <f t="shared" si="8"/>
@@ -5206,7 +5211,7 @@
       </c>
       <c r="N29" s="38">
         <f t="shared" si="7"/>
-        <v>6719.2677525636382</v>
+        <v>67193.552954637154</v>
       </c>
       <c r="O29" s="50">
         <f t="shared" si="8"/>
@@ -5281,7 +5286,7 @@
       </c>
       <c r="N33" s="19">
         <f>$N$6*C70</f>
-        <v>47034.874267945466</v>
+        <v>470354.87068246008</v>
       </c>
       <c r="O33" s="41">
         <f>$O$6*C70</f>
@@ -5309,7 +5314,7 @@
       </c>
       <c r="N34" s="32">
         <f t="shared" ref="N34:N41" si="11">$N$6*C71</f>
-        <v>44795.118350424258</v>
+        <v>447957.01969758107</v>
       </c>
       <c r="O34" s="46">
         <f t="shared" ref="O34:O41" si="12">$O$6*C71</f>
@@ -5337,7 +5342,7 @@
       </c>
       <c r="N35" s="32">
         <f t="shared" si="11"/>
-        <v>38075.850597860619</v>
+        <v>380763.46674294391</v>
       </c>
       <c r="O35" s="46">
         <f t="shared" si="12"/>
@@ -5365,7 +5370,7 @@
       </c>
       <c r="N36" s="32">
         <f t="shared" si="11"/>
-        <v>20157.803257690914</v>
+        <v>201580.65886391146</v>
       </c>
       <c r="O36" s="46">
         <f t="shared" si="12"/>
@@ -5393,7 +5398,7 @@
       </c>
       <c r="N37" s="32">
         <f t="shared" si="11"/>
-        <v>17918.047340169702</v>
+        <v>179182.80787903242</v>
       </c>
       <c r="O37" s="46">
         <f t="shared" si="12"/>
@@ -5421,7 +5426,7 @@
       </c>
       <c r="N38" s="32">
         <f t="shared" si="11"/>
-        <v>15678.291422648492</v>
+        <v>156784.95689415338</v>
       </c>
       <c r="O38" s="46">
         <f t="shared" si="12"/>
@@ -5449,7 +5454,7 @@
       </c>
       <c r="N39" s="32">
         <f t="shared" si="11"/>
-        <v>13438.535505127276</v>
+        <v>134387.10590927431</v>
       </c>
       <c r="O39" s="46">
         <f t="shared" si="12"/>
@@ -5477,7 +5482,7 @@
       </c>
       <c r="N40" s="32">
         <f t="shared" si="11"/>
-        <v>13438.535505127276</v>
+        <v>134387.10590927431</v>
       </c>
       <c r="O40" s="46">
         <f t="shared" si="12"/>
@@ -5505,7 +5510,7 @@
       </c>
       <c r="N41" s="33">
         <f t="shared" si="11"/>
-        <v>11198.779587606065</v>
+        <v>111989.25492439527</v>
       </c>
       <c r="O41" s="42">
         <f t="shared" si="12"/>
@@ -5896,7 +5901,7 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5969,7 +5974,7 @@
       </c>
       <c r="N3" s="19">
         <f>D14*POWER(C3,D15)*C4*C5</f>
-        <v>14.801811709875658</v>
+        <v>148.02004557306537</v>
       </c>
       <c r="O3" s="19">
         <f>E14*POWER(C3,E15)*C4*C5</f>
@@ -5997,7 +6002,7 @@
       </c>
       <c r="N4" s="13">
         <f>N3*C3</f>
-        <v>741911.20833409764</v>
+        <v>7419208.7442587558</v>
       </c>
       <c r="O4" s="13">
         <f>O3*C3</f>
@@ -6026,7 +6031,7 @@
       </c>
       <c r="N6" s="13">
         <f>H3*N3</f>
-        <v>148373.3605797936</v>
+        <v>1483752.9368244074</v>
       </c>
       <c r="O6" s="13">
         <f>H3*O3</f>
@@ -6079,7 +6084,7 @@
       </c>
       <c r="N13" s="36">
         <f>$N$6*C46</f>
-        <v>38577.073750746342</v>
+        <v>385775.76357434597</v>
       </c>
       <c r="O13" s="44">
         <f>$O$6*C46</f>
@@ -6094,7 +6099,7 @@
         <v>17302</v>
       </c>
       <c r="D14" s="19">
-        <v>38377</v>
+        <v>383775</v>
       </c>
       <c r="E14" s="41">
         <v>1734.9</v>
@@ -6108,7 +6113,7 @@
       </c>
       <c r="N14" s="32">
         <f>$N$6*D54</f>
-        <v>15430.829500298536</v>
+        <v>154310.30542973839</v>
       </c>
       <c r="O14" s="46">
         <f>$O$6*D54</f>
@@ -6137,7 +6142,7 @@
       </c>
       <c r="N15" s="32">
         <f>$N$6*D55</f>
-        <v>10801.580650208974</v>
+        <v>108017.21380081687</v>
       </c>
       <c r="O15" s="46">
         <f>$O$6*D55</f>
@@ -6154,7 +6159,7 @@
       </c>
       <c r="N16" s="32">
         <f>$N$6*D56</f>
-        <v>9644.2684376865855</v>
+        <v>96443.940893586492</v>
       </c>
       <c r="O16" s="46">
         <f>$O$6*D56</f>
@@ -6172,7 +6177,7 @@
       </c>
       <c r="N17" s="32">
         <f>$N$6*D57</f>
-        <v>1928.853687537317</v>
+        <v>19288.788178717299</v>
       </c>
       <c r="O17" s="46">
         <f>$O$6*D57</f>
@@ -6194,7 +6199,7 @@
       </c>
       <c r="N18" s="32">
         <f>$N$6*D58</f>
-        <v>771.54147501492685</v>
+        <v>7715.5152714869191</v>
       </c>
       <c r="O18" s="46">
         <f>$O$6*D58</f>
@@ -6223,7 +6228,7 @@
       </c>
       <c r="N19" s="37">
         <f>$N$6*C47</f>
-        <v>34125.872933352533</v>
+        <v>341263.17546961375</v>
       </c>
       <c r="O19" s="48">
         <f>$O$6*C47</f>
@@ -6246,15 +6251,15 @@
         <v>50</v>
       </c>
       <c r="M20" s="45">
-        <f>$M$6*D61</f>
+        <f t="shared" ref="M20:M25" si="1">$M$6*D61</f>
         <v>50901.536014582154</v>
       </c>
       <c r="N20" s="32">
-        <f>$N$6*D61</f>
-        <v>11261.538068006335</v>
+        <f t="shared" ref="N20:N25" si="2">$N$6*D61</f>
+        <v>112616.84790497254</v>
       </c>
       <c r="O20" s="46">
-        <f>$O$6*D61</f>
+        <f t="shared" ref="O20:O25" si="3">$O$6*D61</f>
         <v>33916.850114473091</v>
       </c>
     </row>
@@ -6274,15 +6279,15 @@
         <v>51</v>
       </c>
       <c r="M21" s="45">
-        <f>$M$6*D62</f>
+        <f t="shared" si="1"/>
         <v>33934.357343054762</v>
       </c>
       <c r="N21" s="32">
-        <f>$N$6*D62</f>
-        <v>7507.692045337556</v>
+        <f t="shared" si="2"/>
+        <v>75077.898603315014</v>
       </c>
       <c r="O21" s="46">
-        <f>$O$6*D62</f>
+        <f t="shared" si="3"/>
         <v>22611.233409648721</v>
       </c>
     </row>
@@ -6301,15 +6306,15 @@
         <v>52</v>
       </c>
       <c r="M22" s="45">
-        <f>$M$6*D63</f>
+        <f t="shared" si="1"/>
         <v>29306.944978092753</v>
       </c>
       <c r="N22" s="32">
-        <f>$N$6*D63</f>
-        <v>6483.9158573369805</v>
+        <f t="shared" si="2"/>
+        <v>64840.003339226612</v>
       </c>
       <c r="O22" s="46">
-        <f>$O$6*D63</f>
+        <f t="shared" si="3"/>
         <v>19527.88339924208</v>
       </c>
     </row>
@@ -6328,15 +6333,15 @@
         <v>53</v>
       </c>
       <c r="M23" s="45">
-        <f>$M$6*D64</f>
+        <f t="shared" si="1"/>
         <v>18509.649459848053</v>
       </c>
       <c r="N23" s="32">
-        <f>$N$6*D64</f>
-        <v>4095.1047520023035</v>
+        <f t="shared" si="2"/>
+        <v>40951.581056353643</v>
       </c>
       <c r="O23" s="46">
-        <f>$O$6*D64</f>
+        <f t="shared" si="3"/>
         <v>12333.400041626575</v>
       </c>
     </row>
@@ -6355,15 +6360,15 @@
         <v>54</v>
       </c>
       <c r="M24" s="45">
-        <f>$M$6*D65</f>
+        <f t="shared" si="1"/>
         <v>13882.237094886039</v>
       </c>
       <c r="N24" s="32">
-        <f>$N$6*D65</f>
-        <v>3071.3285640017275</v>
+        <f t="shared" si="2"/>
+        <v>30713.685792265234</v>
       </c>
       <c r="O24" s="46">
-        <f>$O$6*D65</f>
+        <f t="shared" si="3"/>
         <v>9250.050031219931</v>
       </c>
     </row>
@@ -6382,15 +6387,15 @@
         <v>55</v>
       </c>
       <c r="M25" s="45">
-        <f>$M$6*D66</f>
+        <f t="shared" si="1"/>
         <v>7712.3539416033564</v>
       </c>
       <c r="N25" s="32">
-        <f>$N$6*D66</f>
-        <v>1706.2936466676267</v>
+        <f t="shared" si="2"/>
+        <v>17063.158773480689</v>
       </c>
       <c r="O25" s="46">
-        <f>$O$6*D66</f>
+        <f t="shared" si="3"/>
         <v>5138.9166840110738</v>
       </c>
     </row>
@@ -6415,7 +6420,7 @@
       </c>
       <c r="N26" s="37">
         <f>$N$6*C48</f>
-        <v>31158.405721756655</v>
+        <v>311588.11673312553</v>
       </c>
       <c r="O26" s="48">
         <f>$O$6*C48</f>
@@ -6433,7 +6438,7 @@
       </c>
       <c r="N27" s="37">
         <f>$N$6*C49</f>
-        <v>26707.204904362847</v>
+        <v>267075.52862839331</v>
       </c>
       <c r="O27" s="48">
         <f>$O$6*C49</f>
@@ -6460,7 +6465,7 @@
       </c>
       <c r="N28" s="37">
         <f>$N$6*C50</f>
-        <v>13353.602452181423</v>
+        <v>133537.76431419665</v>
       </c>
       <c r="O28" s="48">
         <f>$O$6*C50</f>
@@ -6475,7 +6480,7 @@
         <v>7.45</v>
       </c>
       <c r="D29" s="29">
-        <f t="shared" ref="D29:D42" si="1">(C29/$E$28)</f>
+        <f t="shared" ref="D29:D42" si="4">(C29/$E$28)</f>
         <v>1.5391544360703424</v>
       </c>
       <c r="K29" s="17" t="s">
@@ -6488,7 +6493,7 @@
       </c>
       <c r="N29" s="38">
         <f>$N$6*C51</f>
-        <v>4451.2008173938075</v>
+        <v>44512.588104732218</v>
       </c>
       <c r="O29" s="50">
         <f>$O$6*C51</f>
@@ -6503,7 +6508,7 @@
         <v>6.51</v>
       </c>
       <c r="D30" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.3449523998413326</v>
       </c>
       <c r="M30" s="17"/>
@@ -6516,7 +6521,7 @@
         <v>5.52</v>
       </c>
       <c r="D31" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1404204680682268</v>
       </c>
       <c r="K31" s="39" t="s">
@@ -6531,7 +6536,7 @@
         <v>5.26</v>
       </c>
       <c r="D32" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.0867050112389263</v>
       </c>
       <c r="K32" s="17" t="s">
@@ -6547,22 +6552,22 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="D33" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.95241636916567507</v>
       </c>
       <c r="K33" s="15" t="s">
         <v>13</v>
       </c>
       <c r="M33" s="21">
-        <f>$M$6*C70</f>
+        <f t="shared" ref="M33:M41" si="5">$M$6*C70</f>
         <v>140834.28936840908</v>
       </c>
       <c r="N33" s="19">
-        <f>$N$6*C70</f>
-        <v>31158.405721756655</v>
+        <f t="shared" ref="N33:N41" si="6">$N$6*C70</f>
+        <v>311588.11673312553</v>
       </c>
       <c r="O33" s="41">
-        <f>$O$6*C70</f>
+        <f t="shared" ref="O33:O41" si="7">$O$6*C70</f>
         <v>93841.087273245677</v>
       </c>
     </row>
@@ -6574,22 +6579,22 @@
         <v>4.57</v>
       </c>
       <c r="D34" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.94415245273039805</v>
       </c>
       <c r="K34" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M34" s="45">
-        <f>$M$6*C71</f>
+        <f t="shared" si="5"/>
         <v>134127.89463658011</v>
       </c>
       <c r="N34" s="32">
-        <f>$N$6*C71</f>
-        <v>29674.672115958721</v>
+        <f t="shared" si="6"/>
+        <v>296750.58736488147</v>
       </c>
       <c r="O34" s="46">
-        <f>$O$6*C71</f>
+        <f t="shared" si="7"/>
         <v>89372.4640697578</v>
       </c>
     </row>
@@ -6601,22 +6606,22 @@
         <v>4.55</v>
       </c>
       <c r="D35" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.94002049451275937</v>
       </c>
       <c r="K35" s="15" t="s">
         <v>12</v>
       </c>
       <c r="M35" s="45">
-        <f>$M$6*C72</f>
+        <f t="shared" si="5"/>
         <v>114008.71044109309</v>
       </c>
       <c r="N35" s="32">
-        <f>$N$6*C72</f>
-        <v>25223.471298564913</v>
+        <f t="shared" si="6"/>
+        <v>252237.99926014928</v>
       </c>
       <c r="O35" s="46">
-        <f>$O$6*C72</f>
+        <f t="shared" si="7"/>
         <v>75966.594459294138</v>
       </c>
     </row>
@@ -6628,22 +6633,22 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="D36" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.88217307946582035</v>
       </c>
       <c r="K36" s="15" t="s">
         <v>14</v>
       </c>
       <c r="M36" s="45">
-        <f>$M$6*C73</f>
+        <f t="shared" si="5"/>
         <v>60357.552586461039</v>
       </c>
       <c r="N36" s="32">
-        <f>$N$6*C73</f>
-        <v>13353.602452181423</v>
+        <f t="shared" si="6"/>
+        <v>133537.76431419665</v>
       </c>
       <c r="O36" s="46">
-        <f>$O$6*C73</f>
+        <f t="shared" si="7"/>
         <v>40217.608831391008</v>
       </c>
     </row>
@@ -6655,22 +6660,22 @@
         <v>3.78</v>
       </c>
       <c r="D37" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.78094010313367701</v>
       </c>
       <c r="K37" s="15" t="s">
         <v>15</v>
       </c>
       <c r="M37" s="45">
-        <f>$M$6*C74</f>
+        <f t="shared" si="5"/>
         <v>53651.157854632038</v>
       </c>
       <c r="N37" s="32">
-        <f>$N$6*C74</f>
-        <v>11869.868846383488</v>
+        <f t="shared" si="6"/>
+        <v>118700.2349459526</v>
       </c>
       <c r="O37" s="46">
-        <f>$O$6*C74</f>
+        <f t="shared" si="7"/>
         <v>35748.985627903123</v>
       </c>
     </row>
@@ -6682,22 +6687,22 @@
         <v>3.47</v>
       </c>
       <c r="D38" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.71689475076028031</v>
       </c>
       <c r="K38" s="15" t="s">
         <v>16</v>
       </c>
       <c r="M38" s="45">
-        <f>$M$6*C75</f>
+        <f t="shared" si="5"/>
         <v>46944.763122803037</v>
       </c>
       <c r="N38" s="32">
-        <f>$N$6*C75</f>
-        <v>10386.135240585554</v>
+        <f t="shared" si="6"/>
+        <v>103862.70557770853</v>
       </c>
       <c r="O38" s="46">
-        <f>$O$6*C75</f>
+        <f t="shared" si="7"/>
         <v>31280.362424415231</v>
       </c>
     </row>
@@ -6709,22 +6714,22 @@
         <v>3.39</v>
       </c>
       <c r="D39" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.70036691788972627</v>
       </c>
       <c r="K39" s="15" t="s">
         <v>19</v>
       </c>
       <c r="M39" s="45">
-        <f>$M$6*C76</f>
+        <f t="shared" si="5"/>
         <v>40238.368390974028</v>
       </c>
       <c r="N39" s="32">
-        <f>$N$6*C76</f>
-        <v>8902.401634787615</v>
+        <f t="shared" si="6"/>
+        <v>89025.176209464436</v>
       </c>
       <c r="O39" s="46">
-        <f>$O$6*C76</f>
+        <f t="shared" si="7"/>
         <v>26811.739220927338</v>
       </c>
     </row>
@@ -6736,22 +6741,22 @@
         <v>3.04</v>
       </c>
       <c r="D40" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.62805764908105244</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>17</v>
       </c>
       <c r="M40" s="45">
-        <f>$M$6*C77</f>
+        <f t="shared" si="5"/>
         <v>40238.368390974028</v>
       </c>
       <c r="N40" s="32">
-        <f>$N$6*C77</f>
-        <v>8902.401634787615</v>
+        <f t="shared" si="6"/>
+        <v>89025.176209464436</v>
       </c>
       <c r="O40" s="46">
-        <f>$O$6*C77</f>
+        <f t="shared" si="7"/>
         <v>26811.739220927338</v>
       </c>
     </row>
@@ -6763,22 +6768,22 @@
         <v>2.91</v>
       </c>
       <c r="D41" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.60119992066640227</v>
       </c>
       <c r="K41" s="15" t="s">
         <v>18</v>
       </c>
       <c r="M41" s="22">
-        <f>$M$6*C78</f>
+        <f t="shared" si="5"/>
         <v>33531.973659145027</v>
       </c>
       <c r="N41" s="33">
-        <f>$N$6*C78</f>
-        <v>7418.6680289896804</v>
+        <f t="shared" si="6"/>
+        <v>74187.646841220369</v>
       </c>
       <c r="O41" s="42">
-        <f>$O$6*C78</f>
+        <f t="shared" si="7"/>
         <v>22343.11601743945</v>
       </c>
     </row>
@@ -6790,7 +6795,7 @@
         <v>1.91</v>
       </c>
       <c r="D42" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.39460200978447701</v>
       </c>
     </row>
@@ -6883,7 +6888,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D55" s="27">
-        <f t="shared" ref="D55:D58" si="2">C55*$C$46</f>
+        <f t="shared" ref="D55:D58" si="8">C55*$C$46</f>
         <v>7.2800000000000004E-2</v>
       </c>
     </row>
@@ -6895,7 +6900,7 @@
         <v>0.25</v>
       </c>
       <c r="D56" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
@@ -6907,7 +6912,7 @@
         <v>0.05</v>
       </c>
       <c r="D57" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.3000000000000001E-2</v>
       </c>
     </row>
@@ -6919,7 +6924,7 @@
         <v>0.02</v>
       </c>
       <c r="D58" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.2000000000000006E-3</v>
       </c>
     </row>
@@ -6951,7 +6956,7 @@
         <v>0.22</v>
       </c>
       <c r="D62" s="27">
-        <f t="shared" ref="D62:D66" si="3">C62*$C$47</f>
+        <f t="shared" ref="D62:D66" si="9">C62*$C$47</f>
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
@@ -6963,7 +6968,7 @@
         <v>0.19</v>
       </c>
       <c r="D63" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
@@ -6975,7 +6980,7 @@
         <v>0.12</v>
       </c>
       <c r="D64" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.76E-2</v>
       </c>
     </row>
@@ -6987,7 +6992,7 @@
         <v>0.09</v>
       </c>
       <c r="D65" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.07E-2</v>
       </c>
     </row>
@@ -6999,7 +7004,7 @@
         <v>0.05</v>
       </c>
       <c r="D66" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1500000000000002E-2</v>
       </c>
     </row>

</xml_diff>